<commit_message>
Correcção da forma leitura
</commit_message>
<xml_diff>
--- a/Parser/Constantes_e_Strings-Core.xlsx
+++ b/Parser/Constantes_e_Strings-Core.xlsx
@@ -52,9 +52,6 @@
     <t>Observações</t>
   </si>
   <si>
-    <t>"a", 123, etc…</t>
-  </si>
-  <si>
     <t>"String", 123, etc..</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>A data corresponde ao que vai ser apresentado na forma begin, por defeito para portugues é fim</t>
+  </si>
+  <si>
+    <t>"a"</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +538,7 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -564,11 +564,11 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -579,13 +579,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacao para a nova versao e formas
</commit_message>
<xml_diff>
--- a/Parser/Constantes_e_Strings-Core.xlsx
+++ b/Parser/Constantes_e_Strings-Core.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Constantes e Strings" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Nodes</t>
   </si>
@@ -40,52 +40,95 @@
     <t>"data:"</t>
   </si>
   <si>
-    <t>"inicio"</t>
-  </si>
-  <si>
     <t>"fim"</t>
   </si>
   <si>
-    <t>"name:"</t>
-  </si>
-  <si>
     <t>Observações</t>
   </si>
   <si>
-    <t>"String", 123, etc..</t>
-  </si>
-  <si>
-    <t>Na data corresponde ao texto ou valor a ser apresentado como output</t>
+    <t>A data corresponde ao que vai ser apresentado na forma begin, por defeito para portugues é fim</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>If</t>
+  </si>
+  <si>
+    <t>Join</t>
+  </si>
+  <si>
+    <t>"uuid"</t>
+  </si>
+  <si>
+    <t>caso seja nó de inicio do grafo não existe, caso seja inicio de função "funcao(parametros)"</t>
+  </si>
+  <si>
+    <t>A data corresponde ao que vai ser apresentado na forma begin</t>
+  </si>
+  <si>
+    <t>Expressões "a = 1",b = "func(1)", "a = a +1", "func()</t>
+  </si>
+  <si>
+    <t>O data corresponde à expressão que vai ser validada</t>
+  </si>
+  <si>
+    <t>Expressões "a * 1" "a"</t>
+  </si>
+  <si>
+    <t>Expressões com operadores relacionais "a == b", "b != c"</t>
+  </si>
+  <si>
+    <t>1,2, etc (Sendo que este valor é único)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Na data corresponde ao texto ou valor a ser guardado, pelo input do utilizado e o </t>
+      <t>O data corresponde à expressão de retorno,</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>name a variável na memória</t>
+      <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>A data corresponde ao que vai ser apresentado na forma begin, por defeito para portugues é inicio</t>
-  </si>
-  <si>
-    <t>A data corresponde ao que vai ser apresentado na forma begin, por defeito para portugues é fim</t>
-  </si>
-  <si>
-    <t>"a"</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>não sendo possíveis atribuições</t>
+    </r>
+  </si>
+  <si>
+    <t>Na data corresponde ao à expressão a ser apresentado como output, não sendo possíveis atribuições</t>
+  </si>
+  <si>
+    <t>O data corresponde à expressão a ser validada, sendo que somente são válidos operações com operadores lógicos, não sendo possíveis atribuções</t>
+  </si>
+  <si>
+    <t>Variáveis "a"</t>
+  </si>
+  <si>
+    <t>Na data corresponde ao texto ou valor a ser guardado na variável, pelo input do utilizado</t>
+  </si>
+  <si>
+    <t>Expressões b = "func(1)", "a nome(1)", "func()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +170,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,14 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -177,10 +230,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,106 +546,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F6"/>
+  <dimension ref="B1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="109.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="133.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7" t="s">
-        <v>16</v>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>